<commit_message>
modified the actor update algorithm, now converges much faster but performance is still rather bad
</commit_message>
<xml_diff>
--- a/Robot RL2/Tuning History.xlsx
+++ b/Robot RL2/Tuning History.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="108" windowWidth="15300" windowHeight="8760"/>
+    <workbookView xWindow="0" yWindow="108" windowWidth="15300" windowHeight="8760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -55,6 +55,117 @@
   </si>
   <si>
     <t>Trial 6</t>
+  </si>
+  <si>
+    <t>nrbf X</t>
+  </si>
+  <si>
+    <t>nrbf Y</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>ntrials</t>
+  </si>
+  <si>
+    <t>alpha a</t>
+  </si>
+  <si>
+    <t>alpha c</t>
+  </si>
+  <si>
+    <t>var rand</t>
+  </si>
+  <si>
+    <t>exp steps</t>
+  </si>
+  <si>
+    <t>09-07 PM</t>
+  </si>
+  <si>
+    <t>quadratic</t>
+  </si>
+  <si>
+    <t>almost (refer to fig)</t>
+  </si>
+  <si>
+    <t>Result (1-10)</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>not converged</t>
+  </si>
+  <si>
+    <t>q1</t>
+  </si>
+  <si>
+    <t>q2</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>converge?</t>
+  </si>
+  <si>
+    <t>conv steps</t>
+  </si>
+  <si>
+    <t>performance</t>
+  </si>
+  <si>
+    <t>Trial 7</t>
+  </si>
+  <si>
+    <t>Trial 8</t>
+  </si>
+  <si>
+    <t>Trial 9</t>
+  </si>
+  <si>
+    <t>Trial 10</t>
+  </si>
+  <si>
+    <t>Trial 11</t>
+  </si>
+  <si>
+    <t>Trial 12</t>
+  </si>
+  <si>
+    <t>uSat</t>
+  </si>
+  <si>
+    <t>bad</t>
+  </si>
+  <si>
+    <t>11-12 AM</t>
+  </si>
+  <si>
+    <t>cost fun</t>
+  </si>
+  <si>
+    <t>remark</t>
+  </si>
+  <si>
+    <t>12-57 PM</t>
+  </si>
+  <si>
+    <t>zdotulim</t>
+  </si>
+  <si>
+    <t>zdotllim</t>
+  </si>
+  <si>
+    <t>rather bad</t>
   </si>
 </sst>
 </file>
@@ -78,15 +189,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -94,11 +211,194 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -112,6 +412,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,14 +737,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" customWidth="1"/>
     <col min="4" max="4" width="19.44140625" customWidth="1"/>
     <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
@@ -466,8 +788,12 @@
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="C3" s="2">
+        <v>42104</v>
+      </c>
+      <c r="D3" s="2">
+        <v>42107</v>
+      </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -488,8 +814,12 @@
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -510,7 +840,9 @@
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -532,7 +864,9 @@
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -552,9 +886,11 @@
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="C7" s="1">
+        <v>6</v>
+      </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -576,7 +912,9 @@
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -762,13 +1100,525 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:M25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B1" s="24"/>
+      <c r="C1" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B2" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9">
+        <v>42107</v>
+      </c>
+      <c r="D2" s="9">
+        <v>42107</v>
+      </c>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="16"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="18"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="16"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="11">
+        <v>300</v>
+      </c>
+      <c r="D5" s="11">
+        <v>500</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="20"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="11">
+        <v>40</v>
+      </c>
+      <c r="D6" s="11">
+        <v>40</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="20"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="11">
+        <v>30</v>
+      </c>
+      <c r="D7" s="11">
+        <v>40</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="20"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="12">
+        <v>6.9999999999999999E-6</v>
+      </c>
+      <c r="D8" s="12">
+        <v>6.9999999999999999E-6</v>
+      </c>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="20"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="12">
+        <v>6.9999999999999997E-7</v>
+      </c>
+      <c r="D9" s="12">
+        <v>2.9999999999999999E-7</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="20"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="D10" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="20"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="20"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="12">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D12" s="12">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="20"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="11">
+        <v>3</v>
+      </c>
+      <c r="D13" s="11">
+        <v>3</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="20"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B14" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="12">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D14" s="12">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="20"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B15" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="12">
+        <v>-6.9889999999999997E-5</v>
+      </c>
+      <c r="D15" s="12">
+        <v>-6.9889999999999997E-5</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="20"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B16" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="12">
+        <v>-4.2529999999999998E-3</v>
+      </c>
+      <c r="D16" s="12">
+        <v>-4.2529999999999998E-3</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="20"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="12">
+        <v>20000000</v>
+      </c>
+      <c r="D17" s="12">
+        <v>10000000</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="20"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="12">
+        <v>10000000</v>
+      </c>
+      <c r="D18" s="12">
+        <v>10000000</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="20"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B19" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="D19" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="18"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B20" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="20"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B21" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="20"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B22" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="20"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B23" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="20"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B24" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="20"/>
+    </row>
+    <row r="25" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="22"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
RL2 works, but still required supervision and manual on traininig tuning
</commit_message>
<xml_diff>
--- a/Robot RL2/Tuning History.xlsx
+++ b/Robot RL2/Tuning History.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="76">
   <si>
     <t>Name</t>
   </si>
@@ -166,6 +166,84 @@
   </si>
   <si>
     <t>rather bad</t>
+  </si>
+  <si>
+    <t>remove the randn from the actor updates for few starting iterations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a1 = 3e-06; a2 = 0.05; </t>
+  </si>
+  <si>
+    <t>c1 = 0.1; c2 = 0.7;</t>
+  </si>
+  <si>
+    <t>the first 30-40 trials are showing promising result. Afterwards, the trajectory deviates from the reference greatly</t>
+  </si>
+  <si>
+    <t>critic init</t>
+  </si>
+  <si>
+    <t xml:space="preserve">about 1 PM </t>
+  </si>
+  <si>
+    <t>14-51 PM</t>
+  </si>
+  <si>
+    <t>BAD</t>
+  </si>
+  <si>
+    <t>pessimistic initialization is not effective after all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a1 = 4e-06; a2 = 0.05; </t>
+  </si>
+  <si>
+    <t>c1 = 0.4; c2 = 0.7;</t>
+  </si>
+  <si>
+    <t>gamma</t>
+  </si>
+  <si>
+    <t>15-40 PM</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>moderate</t>
+  </si>
+  <si>
+    <t>the critic and actor got stuck at local optima at the end of the trial, perhaps it is better to increase the varRand at  that moment. Furthermore, the gamma is also interested to tweak</t>
+  </si>
+  <si>
+    <t>tried switching actor parameter update rule from with to no Delta_u term. Can cause instability at the switching. Probably I set the varRand too large.</t>
+  </si>
+  <si>
+    <t>terrible, unstable</t>
+  </si>
+  <si>
+    <t>10-52 AM</t>
+  </si>
+  <si>
+    <t>16-38 PM</t>
+  </si>
+  <si>
+    <t>better than before, but still not optimal</t>
+  </si>
+  <si>
+    <t>tuned the varRand, idxRand, alpha_a1 during the trials</t>
+  </si>
+  <si>
+    <t>&gt;300</t>
+  </si>
+  <si>
+    <t>17-49 PM</t>
+  </si>
+  <si>
+    <t>bad, not even better than the nominal one</t>
+  </si>
+  <si>
+    <t>reducing the gamma (discount rate) gives a slower convergence and poorer performance. Need to check if the value is increased and/or decreased</t>
   </si>
 </sst>
 </file>
@@ -398,7 +476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -434,6 +512,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1100,16 +1180,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M25"/>
+  <dimension ref="B1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.3">
@@ -1158,12 +1240,24 @@
       <c r="D2" s="9">
         <v>42107</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
+      <c r="E2" s="27">
+        <v>42108</v>
+      </c>
+      <c r="F2" s="27">
+        <v>42108</v>
+      </c>
+      <c r="G2" s="27">
+        <v>42108</v>
+      </c>
+      <c r="H2" s="27">
+        <v>42109</v>
+      </c>
+      <c r="I2" s="27">
+        <v>42109</v>
+      </c>
+      <c r="J2" s="27">
+        <v>42109</v>
+      </c>
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
       <c r="M2" s="16"/>
@@ -1178,12 +1272,24 @@
       <c r="D3" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
+      <c r="E3" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
       <c r="M3" s="18"/>
@@ -1214,12 +1320,24 @@
       <c r="D5" s="11">
         <v>500</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
+      <c r="E5" s="11">
+        <v>500</v>
+      </c>
+      <c r="F5" s="11">
+        <v>500</v>
+      </c>
+      <c r="G5" s="11">
+        <v>500</v>
+      </c>
+      <c r="H5" s="11">
+        <v>500</v>
+      </c>
+      <c r="I5" s="11">
+        <v>500</v>
+      </c>
+      <c r="J5" s="11">
+        <v>500</v>
+      </c>
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
       <c r="M5" s="20"/>
@@ -1234,12 +1352,24 @@
       <c r="D6" s="11">
         <v>40</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
+      <c r="E6" s="11">
+        <v>40</v>
+      </c>
+      <c r="F6" s="11">
+        <v>40</v>
+      </c>
+      <c r="G6" s="11">
+        <v>40</v>
+      </c>
+      <c r="H6" s="11">
+        <v>40</v>
+      </c>
+      <c r="I6" s="11">
+        <v>40</v>
+      </c>
+      <c r="J6" s="11">
+        <v>40</v>
+      </c>
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
       <c r="M6" s="20"/>
@@ -1254,12 +1384,24 @@
       <c r="D7" s="11">
         <v>40</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
+      <c r="E7" s="11">
+        <v>40</v>
+      </c>
+      <c r="F7" s="11">
+        <v>40</v>
+      </c>
+      <c r="G7" s="11">
+        <v>40</v>
+      </c>
+      <c r="H7" s="11">
+        <v>40</v>
+      </c>
+      <c r="I7" s="11">
+        <v>40</v>
+      </c>
+      <c r="J7" s="11">
+        <v>40</v>
+      </c>
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
       <c r="M7" s="20"/>
@@ -1274,12 +1416,24 @@
       <c r="D8" s="12">
         <v>6.9999999999999999E-6</v>
       </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
+      <c r="E8" s="12">
+        <v>3.9999999999999998E-7</v>
+      </c>
+      <c r="F8" s="12">
+        <v>3.9999999999999998E-7</v>
+      </c>
+      <c r="G8" s="12">
+        <v>4.9999999999999998E-7</v>
+      </c>
+      <c r="H8" s="12">
+        <v>4.9999999999999998E-7</v>
+      </c>
+      <c r="I8" s="12">
+        <v>4.9999999999999998E-7</v>
+      </c>
+      <c r="J8" s="12">
+        <v>4.9999999999999998E-7</v>
+      </c>
       <c r="K8" s="11"/>
       <c r="L8" s="11"/>
       <c r="M8" s="20"/>
@@ -1294,12 +1448,24 @@
       <c r="D9" s="12">
         <v>2.9999999999999999E-7</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
+      <c r="E9" s="12">
+        <v>3.9999999999999998E-7</v>
+      </c>
+      <c r="F9" s="12">
+        <v>3.9999999999999998E-7</v>
+      </c>
+      <c r="G9" s="12">
+        <v>4.9999999999999998E-7</v>
+      </c>
+      <c r="H9" s="12">
+        <v>4.9999999999999998E-7</v>
+      </c>
+      <c r="I9" s="12">
+        <v>4.9999999999999998E-7</v>
+      </c>
+      <c r="J9" s="12">
+        <v>4.9999999999999998E-7</v>
+      </c>
       <c r="K9" s="11"/>
       <c r="L9" s="11"/>
       <c r="M9" s="20"/>
@@ -1314,12 +1480,24 @@
       <c r="D10" s="11">
         <v>0.05</v>
       </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
+      <c r="E10" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="K10" s="11"/>
       <c r="L10" s="11"/>
       <c r="M10" s="20"/>
@@ -1334,12 +1512,24 @@
       <c r="D11" s="11">
         <v>0.7</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
+      <c r="E11" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>52</v>
+      </c>
       <c r="K11" s="11"/>
       <c r="L11" s="11"/>
       <c r="M11" s="20"/>
@@ -1354,12 +1544,24 @@
       <c r="D12" s="12">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
+      <c r="E12" s="12">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="F12" s="12">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="G12" s="12">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="H12" s="12">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="I12" s="12">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="J12" s="12">
+        <v>2.0000000000000001E-4</v>
+      </c>
       <c r="K12" s="11"/>
       <c r="L12" s="11"/>
       <c r="M12" s="20"/>
@@ -1374,12 +1576,24 @@
       <c r="D13" s="11">
         <v>3</v>
       </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
+      <c r="E13" s="11">
+        <v>3</v>
+      </c>
+      <c r="F13" s="11">
+        <v>3</v>
+      </c>
+      <c r="G13" s="11">
+        <v>3</v>
+      </c>
+      <c r="H13" s="11">
+        <v>3</v>
+      </c>
+      <c r="I13" s="11">
+        <v>3</v>
+      </c>
+      <c r="J13" s="11">
+        <v>3</v>
+      </c>
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
       <c r="M13" s="20"/>
@@ -1394,12 +1608,24 @@
       <c r="D14" s="12">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
+      <c r="E14" s="12">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F14" s="12">
+        <v>0.06</v>
+      </c>
+      <c r="G14" s="12">
+        <v>0.06</v>
+      </c>
+      <c r="H14" s="12">
+        <v>0.06</v>
+      </c>
+      <c r="I14" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="J14" s="12">
+        <v>0.01</v>
+      </c>
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
       <c r="M14" s="20"/>
@@ -1414,12 +1640,24 @@
       <c r="D15" s="12">
         <v>-6.9889999999999997E-5</v>
       </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
+      <c r="E15" s="12">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F15" s="12">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G15" s="12">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="H15" s="12">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="I15" s="12">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J15" s="12">
+        <v>4.0000000000000001E-3</v>
+      </c>
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
       <c r="M15" s="20"/>
@@ -1434,122 +1672,194 @@
       <c r="D16" s="12">
         <v>-4.2529999999999998E-3</v>
       </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
+      <c r="E16" s="12">
+        <v>-4.2529999999999998E-3</v>
+      </c>
+      <c r="F16" s="12">
+        <v>-4.2529999999999998E-3</v>
+      </c>
+      <c r="G16" s="12">
+        <v>-4.2529999999999998E-3</v>
+      </c>
+      <c r="H16" s="12">
+        <v>-4.2529999999999998E-3</v>
+      </c>
+      <c r="I16" s="12">
+        <v>-4.2529999999999998E-3</v>
+      </c>
+      <c r="J16" s="12">
+        <v>-4.2529999999999998E-3</v>
+      </c>
       <c r="K16" s="11"/>
       <c r="L16" s="11"/>
       <c r="M16" s="20"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="C17" s="12">
-        <v>20000000</v>
+        <v>0</v>
       </c>
       <c r="D17" s="12">
-        <v>10000000</v>
-      </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="12">
+        <v>-40000</v>
+      </c>
+      <c r="F17" s="12">
+        <v>-40000</v>
+      </c>
+      <c r="G17" s="12">
+        <v>0</v>
+      </c>
+      <c r="H17" s="12">
+        <v>0</v>
+      </c>
+      <c r="I17" s="12">
+        <v>0</v>
+      </c>
+      <c r="J17" s="12">
+        <v>0</v>
+      </c>
       <c r="K17" s="11"/>
       <c r="L17" s="11"/>
       <c r="M17" s="20"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="C18" s="12">
-        <v>10000000</v>
+        <v>0.97</v>
       </c>
       <c r="D18" s="12">
-        <v>10000000</v>
-      </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
+        <v>0.97</v>
+      </c>
+      <c r="E18" s="12">
+        <v>0.97</v>
+      </c>
+      <c r="F18" s="12">
+        <v>0.97</v>
+      </c>
+      <c r="G18" s="12">
+        <v>0.97</v>
+      </c>
+      <c r="H18" s="12">
+        <v>0.97</v>
+      </c>
+      <c r="I18" s="12">
+        <v>0.97</v>
+      </c>
+      <c r="J18" s="12">
+        <v>0.87</v>
+      </c>
       <c r="K18" s="11"/>
       <c r="L18" s="11"/>
       <c r="M18" s="20"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B19" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="D19" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="18"/>
+      <c r="B19" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="12">
+        <v>20000000</v>
+      </c>
+      <c r="D19" s="12">
+        <v>10000000</v>
+      </c>
+      <c r="E19" s="12">
+        <v>10000000</v>
+      </c>
+      <c r="F19" s="12">
+        <v>10000000</v>
+      </c>
+      <c r="G19" s="12">
+        <v>10000000</v>
+      </c>
+      <c r="H19" s="12">
+        <v>10000000</v>
+      </c>
+      <c r="I19" s="12">
+        <v>10000000</v>
+      </c>
+      <c r="J19" s="12">
+        <v>10000000</v>
+      </c>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="20"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
+      <c r="B20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="12">
+        <v>10000000</v>
+      </c>
+      <c r="D20" s="12">
+        <v>10000000</v>
+      </c>
+      <c r="E20" s="12">
+        <v>10000000</v>
+      </c>
+      <c r="F20" s="12">
+        <v>10000000</v>
+      </c>
+      <c r="G20" s="12">
+        <v>10000000</v>
+      </c>
+      <c r="H20" s="12">
+        <v>10000000</v>
+      </c>
+      <c r="I20" s="12">
+        <v>1000000</v>
+      </c>
+      <c r="J20" s="12">
+        <v>1000000</v>
+      </c>
       <c r="K20" s="11"/>
       <c r="L20" s="11"/>
       <c r="M20" s="20"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="20"/>
+      <c r="B21" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="D21" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="E21" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="F21" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="G21" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="H21" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="I21" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="J21" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="18"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>49</v>
-      </c>
+      <c r="B22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
@@ -1562,59 +1872,159 @@
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B23" s="6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
+        <v>26</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="J23" s="11" t="s">
+        <v>63</v>
+      </c>
       <c r="K23" s="11"/>
       <c r="L23" s="11"/>
       <c r="M23" s="20"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
+        <v>34</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="J24" s="11" t="s">
+        <v>74</v>
+      </c>
       <c r="K24" s="11"/>
       <c r="L24" s="11"/>
       <c r="M24" s="20"/>
     </row>
-    <row r="25" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="7" t="s">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B25" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J25" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="20"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B26" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="J26" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="20"/>
+    </row>
+    <row r="27" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C27" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="21" t="s">
+      <c r="D27" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="21"/>
-      <c r="M25" s="22"/>
+      <c r="E27" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" s="21">
+        <v>33</v>
+      </c>
+      <c r="H27" s="21">
+        <v>40</v>
+      </c>
+      <c r="I27" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="J27" s="21">
+        <v>30</v>
+      </c>
+      <c r="K27" s="21"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>